<commit_message>
finished all the merges and collapsed each year
</commit_message>
<xml_diff>
--- a/data/reg_dif_med_results/difmedias_entre_anos_2019x2023.xlsx
+++ b/data/reg_dif_med_results/difmedias_entre_anos_2019x2023.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="938" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="868" uniqueCount="212">
   <si>
     <t/>
   </si>
@@ -114,18 +114,6 @@
     <t>ocupacion1_d13</t>
   </si>
   <si>
-    <t>ocupacion1_d14</t>
-  </si>
-  <si>
-    <t>ocupacion1_d15</t>
-  </si>
-  <si>
-    <t>ocupacion1_d16</t>
-  </si>
-  <si>
-    <t>ocupacion1_d17</t>
-  </si>
-  <si>
     <t>ocupacion1_d18</t>
   </si>
   <si>
@@ -213,22 +201,19 @@
     <t>actividad_economica1_d19</t>
   </si>
   <si>
-    <t>nivel_educativo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the table includes missing values (.n, .o, .v etc.) see the Missing values section in the help file for the Stata command iebaltab for definitions of these values. Significance: ***=.01, **=.05, *=.1. Full user input as written by user: [iebaltab estrato edad limitaciones_fisicas mujer total_personas total_personas_mas_5 nivel_educativo_d* tipo_vivienda_d* ocupacion1_d* actividad_economica1_d* nivel_educativo , groupvar(a2019) control(0) savexlsx(difmedias_entre_anos_2019x2023) replace] </t>
+    <t xml:space="preserve">If the table includes missing values (.n, .o, .v etc.) see the Missing values section in the help file for the Stata command iebaltab for definitions of these values. Significance: ***=.01, **=.05, *=.1. Full user input as written by user: [iebaltab estrato edad limitaciones_fisicas mujer total_personas total_personas_mas_5 nivel_educativo_d* tipo_vivienda_d* ocupacion1_d* actividad_economica1_d* , groupvar(a2019) control(0) savexlsx(difmedias_entre_anos_2019x2023) replace] </t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>15652</t>
-  </si>
-  <si>
-    <t>20668</t>
-  </si>
-  <si>
-    <t>20664</t>
+    <t>15650</t>
+  </si>
+  <si>
+    <t>20666</t>
+  </si>
+  <si>
+    <t>20662</t>
   </si>
   <si>
     <t xml:space="preserve"> (1) </t>
@@ -246,7 +231,7 @@
     <t>(0.009)</t>
   </si>
   <si>
-    <t>38.980</t>
+    <t>38.978</t>
   </si>
   <si>
     <t>(0.092)</t>
@@ -342,159 +327,159 @@
     <t>0.001</t>
   </si>
   <si>
+    <t>0.017</t>
+  </si>
+  <si>
+    <t>0.010</t>
+  </si>
+  <si>
+    <t>0.011</t>
+  </si>
+  <si>
+    <t>0.020</t>
+  </si>
+  <si>
+    <t>0.050</t>
+  </si>
+  <si>
+    <t>0.511</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
     <t>0.005</t>
   </si>
   <si>
+    <t>0.058</t>
+  </si>
+  <si>
+    <t>0.062</t>
+  </si>
+  <si>
+    <t>0.033</t>
+  </si>
+  <si>
+    <t>0.072</t>
+  </si>
+  <si>
+    <t>0.019</t>
+  </si>
+  <si>
+    <t>0.030</t>
+  </si>
+  <si>
+    <t>0.037</t>
+  </si>
+  <si>
+    <t>0.474</t>
+  </si>
+  <si>
+    <t>0.004</t>
+  </si>
+  <si>
+    <t>16740</t>
+  </si>
+  <si>
+    <t>17608</t>
+  </si>
+  <si>
+    <t>13509</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (2) </t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2.642</t>
+  </si>
+  <si>
+    <t>(0.008)</t>
+  </si>
+  <si>
+    <t>39.315</t>
+  </si>
+  <si>
+    <t>(0.574)</t>
+  </si>
+  <si>
+    <t>0.451</t>
+  </si>
+  <si>
+    <t>(0.004)</t>
+  </si>
+  <si>
+    <t>3.788</t>
+  </si>
+  <si>
+    <t>(0.012)</t>
+  </si>
+  <si>
+    <t>3.586</t>
+  </si>
+  <si>
+    <t>0.042</t>
+  </si>
+  <si>
+    <t>0.059</t>
+  </si>
+  <si>
+    <t>0.148</t>
+  </si>
+  <si>
+    <t>0.197</t>
+  </si>
+  <si>
+    <t>0.025</t>
+  </si>
+  <si>
+    <t>0.132</t>
+  </si>
+  <si>
+    <t>0.069</t>
+  </si>
+  <si>
+    <t>0.201</t>
+  </si>
+  <si>
+    <t>0.009</t>
+  </si>
+  <si>
+    <t>0.111</t>
+  </si>
+  <si>
+    <t>0.480</t>
+  </si>
+  <si>
+    <t>0.488</t>
+  </si>
+  <si>
+    <t>0.026</t>
+  </si>
+  <si>
+    <t>0.039</t>
+  </si>
+  <si>
+    <t>0.155</t>
+  </si>
+  <si>
+    <t>0.055</t>
+  </si>
+  <si>
+    <t>0.014</t>
+  </si>
+  <si>
+    <t>0.080</t>
+  </si>
+  <si>
+    <t>0.083</t>
+  </si>
+  <si>
     <t>0.008</t>
   </si>
   <si>
-    <t>0.010</t>
-  </si>
-  <si>
-    <t>0.020</t>
-  </si>
-  <si>
-    <t>0.050</t>
-  </si>
-  <si>
-    <t>0.511</t>
-  </si>
-  <si>
-    <t>0.007</t>
-  </si>
-  <si>
-    <t>0.058</t>
-  </si>
-  <si>
-    <t>0.062</t>
-  </si>
-  <si>
-    <t>0.033</t>
-  </si>
-  <si>
-    <t>0.072</t>
-  </si>
-  <si>
-    <t>0.019</t>
-  </si>
-  <si>
-    <t>0.030</t>
-  </si>
-  <si>
-    <t>0.037</t>
-  </si>
-  <si>
-    <t>0.474</t>
-  </si>
-  <si>
-    <t>0.004</t>
-  </si>
-  <si>
-    <t>0.017</t>
-  </si>
-  <si>
-    <t>6.082</t>
-  </si>
-  <si>
-    <t>(0.017)</t>
-  </si>
-  <si>
-    <t>16748</t>
-  </si>
-  <si>
-    <t>17616</t>
-  </si>
-  <si>
-    <t>13516</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (2) </t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2.642</t>
-  </si>
-  <si>
-    <t>(0.008)</t>
-  </si>
-  <si>
-    <t>39.307</t>
-  </si>
-  <si>
-    <t>(0.574)</t>
-  </si>
-  <si>
-    <t>0.451</t>
-  </si>
-  <si>
-    <t>(0.004)</t>
-  </si>
-  <si>
-    <t>3.789</t>
-  </si>
-  <si>
-    <t>(0.012)</t>
-  </si>
-  <si>
-    <t>3.587</t>
-  </si>
-  <si>
-    <t>0.042</t>
-  </si>
-  <si>
-    <t>0.059</t>
-  </si>
-  <si>
-    <t>0.148</t>
-  </si>
-  <si>
-    <t>0.198</t>
-  </si>
-  <si>
-    <t>0.025</t>
-  </si>
-  <si>
-    <t>0.132</t>
-  </si>
-  <si>
-    <t>0.069</t>
-  </si>
-  <si>
-    <t>0.200</t>
-  </si>
-  <si>
-    <t>0.009</t>
-  </si>
-  <si>
-    <t>0.111</t>
-  </si>
-  <si>
-    <t>0.480</t>
-  </si>
-  <si>
-    <t>0.488</t>
-  </si>
-  <si>
-    <t>0.026</t>
-  </si>
-  <si>
-    <t>0.039</t>
-  </si>
-  <si>
-    <t>0.155</t>
-  </si>
-  <si>
-    <t>0.055</t>
-  </si>
-  <si>
-    <t>0.014</t>
-  </si>
-  <si>
-    <t>0.084</t>
-  </si>
-  <si>
     <t>0.013</t>
   </si>
   <si>
@@ -519,31 +504,28 @@
     <t>0.034</t>
   </si>
   <si>
+    <t>0.068</t>
+  </si>
+  <si>
     <t>0.053</t>
   </si>
   <si>
-    <t>0.329</t>
+    <t>0.328</t>
   </si>
   <si>
     <t>0.041</t>
   </si>
   <si>
-    <t>6.660</t>
-  </si>
-  <si>
-    <t>(0.020)</t>
-  </si>
-  <si>
-    <t>32400</t>
-  </si>
-  <si>
-    <t>38284</t>
-  </si>
-  <si>
-    <t>34184</t>
-  </si>
-  <si>
-    <t>38280</t>
+    <t>32390</t>
+  </si>
+  <si>
+    <t>38274</t>
+  </si>
+  <si>
+    <t>34175</t>
+  </si>
+  <si>
+    <t>38270</t>
   </si>
   <si>
     <t>(2)-(1)</t>
@@ -558,19 +540,19 @@
     <t>0.107***</t>
   </si>
   <si>
-    <t>0.327</t>
+    <t>0.337</t>
   </si>
   <si>
     <t>-0.006***</t>
   </si>
   <si>
-    <t>0.027***</t>
-  </si>
-  <si>
-    <t>0.218***</t>
-  </si>
-  <si>
-    <t>0.147***</t>
+    <t>0.028***</t>
+  </si>
+  <si>
+    <t>0.217***</t>
+  </si>
+  <si>
+    <t>0.146***</t>
   </si>
   <si>
     <t>0.010***</t>
@@ -588,7 +570,7 @@
     <t>-0.004**</t>
   </si>
   <si>
-    <t>0.037***</t>
+    <t>0.038***</t>
   </si>
   <si>
     <t>0.012***</t>
@@ -630,10 +612,7 @@
     <t>0.004***</t>
   </si>
   <si>
-    <t>0.031***</t>
-  </si>
-  <si>
-    <t>0.013***</t>
+    <t>0.063***</t>
   </si>
   <si>
     <t>0.071***</t>
@@ -663,19 +642,13 @@
     <t>0.015***</t>
   </si>
   <si>
-    <t>0.038***</t>
-  </si>
-  <si>
     <t>-0.145***</t>
   </si>
   <si>
     <t>0.008***</t>
   </si>
   <si>
-    <t>0.024***</t>
-  </si>
-  <si>
-    <t>0.578***</t>
+    <t>0.023***</t>
   </si>
 </sst>
 </file>
@@ -719,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -733,19 +706,19 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2">
@@ -756,19 +729,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3">
@@ -776,22 +749,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
@@ -799,22 +772,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5">
@@ -825,13 +798,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -845,22 +818,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
@@ -871,13 +844,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -891,22 +864,22 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9">
@@ -917,13 +890,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -937,22 +910,22 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G10" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11">
@@ -963,13 +936,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -983,22 +956,22 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G12" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13">
@@ -1009,13 +982,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -1029,22 +1002,22 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G14" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15">
@@ -1055,13 +1028,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -1075,22 +1048,22 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -1101,13 +1074,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
@@ -1121,22 +1094,22 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F18" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G18" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19">
@@ -1147,13 +1120,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
         <v>0</v>
@@ -1167,22 +1140,22 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F20" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G20" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21">
@@ -1193,13 +1166,13 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
@@ -1213,22 +1186,22 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F22" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G22" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
@@ -1239,13 +1212,13 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
         <v>0</v>
@@ -1259,22 +1232,22 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F24" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25">
@@ -1285,13 +1258,13 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
         <v>0</v>
@@ -1305,22 +1278,22 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F26" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G26" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27">
@@ -1331,13 +1304,13 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F27" t="s">
         <v>0</v>
@@ -1351,22 +1324,22 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F28" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29">
@@ -1377,13 +1350,13 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
         <v>0</v>
@@ -1397,22 +1370,22 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G30" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31">
@@ -1423,13 +1396,13 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F31" t="s">
         <v>0</v>
@@ -1443,22 +1416,22 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F32" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G32" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33">
@@ -1469,13 +1442,13 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
         <v>0</v>
@@ -1489,22 +1462,22 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E34" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F34" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G34" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35">
@@ -1515,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F35" t="s">
         <v>0</v>
@@ -1535,22 +1508,22 @@
         <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E36" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F36" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G36" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37">
@@ -1561,13 +1534,13 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F37" t="s">
         <v>0</v>
@@ -1581,22 +1554,22 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E38" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G38" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39">
@@ -1607,13 +1580,13 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F39" t="s">
         <v>0</v>
@@ -1627,22 +1600,22 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E40" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F40" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G40" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41">
@@ -1653,13 +1626,13 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F41" t="s">
         <v>0</v>
@@ -1673,22 +1646,22 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E42" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F42" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G42" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43">
@@ -1699,13 +1672,13 @@
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F43" t="s">
         <v>0</v>
@@ -1719,22 +1692,22 @@
         <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F44" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G44" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45">
@@ -1745,13 +1718,13 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F45" t="s">
         <v>0</v>
@@ -1765,22 +1738,22 @@
         <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D46" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F46" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G46" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47">
@@ -1791,13 +1764,13 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
         <v>0</v>
@@ -1811,22 +1784,22 @@
         <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F48" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G48" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49">
@@ -1837,13 +1810,13 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D49" t="s">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F49" t="s">
         <v>0</v>
@@ -1857,22 +1830,22 @@
         <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F50" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G50" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51">
@@ -1883,13 +1856,13 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D51" t="s">
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F51" t="s">
         <v>0</v>
@@ -1903,22 +1876,22 @@
         <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E52" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F52" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G52" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53">
@@ -1929,13 +1902,13 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D53" t="s">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F53" t="s">
         <v>0</v>
@@ -1949,22 +1922,22 @@
         <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E54" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F54" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G54" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55">
@@ -1975,13 +1948,13 @@
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D55" t="s">
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F55" t="s">
         <v>0</v>
@@ -1995,22 +1968,22 @@
         <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F56" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G56" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57">
@@ -2021,13 +1994,13 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D57" t="s">
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F57" t="s">
         <v>0</v>
@@ -2041,22 +2014,22 @@
         <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E58" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F58" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G58" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59">
@@ -2067,13 +2040,13 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D59" t="s">
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F59" t="s">
         <v>0</v>
@@ -2087,22 +2060,22 @@
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F60" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G60" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61">
@@ -2113,13 +2086,13 @@
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D61" t="s">
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F61" t="s">
         <v>0</v>
@@ -2133,22 +2106,22 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E62" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="F62" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G62" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63">
@@ -2159,13 +2132,13 @@
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D63" t="s">
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F63" t="s">
         <v>0</v>
@@ -2179,19 +2152,19 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D64" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E64" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="F64" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G64" t="s">
         <v>199</v>
@@ -2205,13 +2178,13 @@
         <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D65" t="s">
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F65" t="s">
         <v>0</v>
@@ -2225,22 +2198,22 @@
         <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="D66" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E66" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F66" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G66" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67">
@@ -2251,13 +2224,13 @@
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D67" t="s">
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F67" t="s">
         <v>0</v>
@@ -2271,22 +2244,22 @@
         <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D68" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E68" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F68" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G68" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69">
@@ -2297,13 +2270,13 @@
         <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D69" t="s">
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F69" t="s">
         <v>0</v>
@@ -2317,22 +2290,22 @@
         <v>35</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D70" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E70" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F70" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G70" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71">
@@ -2343,13 +2316,13 @@
         <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D71" t="s">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F71" t="s">
         <v>0</v>
@@ -2363,22 +2336,22 @@
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D72" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E72" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F72" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G72" t="s">
-        <v>193</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73">
@@ -2389,13 +2362,13 @@
         <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D73" t="s">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F73" t="s">
         <v>0</v>
@@ -2409,22 +2382,22 @@
         <v>37</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C74" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D74" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E74" t="s">
-        <v>159</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G74" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75">
@@ -2435,13 +2408,13 @@
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D75" t="s">
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F75" t="s">
         <v>0</v>
@@ -2455,22 +2428,22 @@
         <v>38</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D76" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E76" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="F76" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G76" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77">
@@ -2481,13 +2454,13 @@
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D77" t="s">
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F77" t="s">
         <v>0</v>
@@ -2501,22 +2474,22 @@
         <v>39</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C78" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="D78" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E78" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="F78" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G78" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79">
@@ -2527,13 +2500,13 @@
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D79" t="s">
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F79" t="s">
         <v>0</v>
@@ -2547,22 +2520,22 @@
         <v>40</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C80" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D80" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E80" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="F80" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G80" t="s">
-        <v>87</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81">
@@ -2573,13 +2546,13 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D81" t="s">
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F81" t="s">
         <v>0</v>
@@ -2593,22 +2566,22 @@
         <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C82" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="D82" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E82" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="F82" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G82" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83">
@@ -2619,13 +2592,13 @@
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D83" t="s">
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F83" t="s">
         <v>0</v>
@@ -2639,22 +2612,22 @@
         <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E84" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F84" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G84" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85">
@@ -2665,13 +2638,13 @@
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D85" t="s">
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="F85" t="s">
         <v>0</v>
@@ -2685,22 +2658,22 @@
         <v>43</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C86" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D86" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E86" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F86" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G86" t="s">
-        <v>209</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87">
@@ -2711,13 +2684,13 @@
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D87" t="s">
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F87" t="s">
         <v>0</v>
@@ -2731,22 +2704,22 @@
         <v>44</v>
       </c>
       <c r="B88" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C88" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D88" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E88" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="F88" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G88" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89">
@@ -2757,13 +2730,13 @@
         <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D89" t="s">
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F89" t="s">
         <v>0</v>
@@ -2777,22 +2750,22 @@
         <v>45</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D90" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E90" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="F90" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G90" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91">
@@ -2803,13 +2776,13 @@
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D91" t="s">
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F91" t="s">
         <v>0</v>
@@ -2823,22 +2796,22 @@
         <v>46</v>
       </c>
       <c r="B92" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D92" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E92" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="F92" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G92" t="s">
-        <v>213</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93">
@@ -2849,13 +2822,13 @@
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D93" t="s">
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="F93" t="s">
         <v>0</v>
@@ -2869,22 +2842,22 @@
         <v>47</v>
       </c>
       <c r="B94" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C94" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D94" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E94" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="F94" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G94" t="s">
-        <v>87</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95">
@@ -2895,13 +2868,13 @@
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D95" t="s">
         <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F95" t="s">
         <v>0</v>
@@ -2915,22 +2888,22 @@
         <v>48</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C96" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D96" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E96" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="F96" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G96" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
     </row>
     <row r="97">
@@ -2941,13 +2914,13 @@
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D97" t="s">
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F97" t="s">
         <v>0</v>
@@ -2961,22 +2934,22 @@
         <v>49</v>
       </c>
       <c r="B98" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C98" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D98" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E98" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="F98" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G98" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99">
@@ -2987,13 +2960,13 @@
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D99" t="s">
         <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F99" t="s">
         <v>0</v>
@@ -3007,22 +2980,22 @@
         <v>50</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C100" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D100" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E100" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F100" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G100" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
     </row>
     <row r="101">
@@ -3033,13 +3006,13 @@
         <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D101" t="s">
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F101" t="s">
         <v>0</v>
@@ -3053,22 +3026,22 @@
         <v>51</v>
       </c>
       <c r="B102" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C102" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D102" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E102" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="F102" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G102" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103">
@@ -3079,13 +3052,13 @@
         <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D103" t="s">
         <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F103" t="s">
         <v>0</v>
@@ -3099,22 +3072,22 @@
         <v>52</v>
       </c>
       <c r="B104" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C104" t="s">
         <v>116</v>
       </c>
       <c r="D104" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E104" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F104" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G104" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="105">
@@ -3125,13 +3098,13 @@
         <v>0</v>
       </c>
       <c r="C105" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D105" t="s">
         <v>0</v>
       </c>
       <c r="E105" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F105" t="s">
         <v>0</v>
@@ -3145,22 +3118,22 @@
         <v>53</v>
       </c>
       <c r="B106" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C106" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D106" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E106" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="F106" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G106" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107">
@@ -3171,13 +3144,13 @@
         <v>0</v>
       </c>
       <c r="C107" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D107" t="s">
         <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F107" t="s">
         <v>0</v>
@@ -3191,22 +3164,22 @@
         <v>54</v>
       </c>
       <c r="B108" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C108" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="D108" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E108" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="F108" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G108" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109">
@@ -3217,13 +3190,13 @@
         <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D109" t="s">
         <v>0</v>
       </c>
       <c r="E109" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F109" t="s">
         <v>0</v>
@@ -3237,22 +3210,22 @@
         <v>55</v>
       </c>
       <c r="B110" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C110" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D110" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E110" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F110" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G110" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111">
@@ -3263,13 +3236,13 @@
         <v>0</v>
       </c>
       <c r="C111" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D111" t="s">
         <v>0</v>
       </c>
       <c r="E111" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F111" t="s">
         <v>0</v>
@@ -3283,22 +3256,22 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C112" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D112" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E112" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F112" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G112" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="113">
@@ -3309,13 +3282,13 @@
         <v>0</v>
       </c>
       <c r="C113" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D113" t="s">
         <v>0</v>
       </c>
       <c r="E113" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F113" t="s">
         <v>0</v>
@@ -3329,19 +3302,19 @@
         <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C114" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D114" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E114" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="F114" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G114" t="s">
         <v>209</v>
@@ -3355,13 +3328,13 @@
         <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D115" t="s">
         <v>0</v>
       </c>
       <c r="E115" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="F115" t="s">
         <v>0</v>
@@ -3375,22 +3348,22 @@
         <v>58</v>
       </c>
       <c r="B116" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C116" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D116" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E116" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="F116" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G116" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117">
@@ -3401,13 +3374,13 @@
         <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D117" t="s">
         <v>0</v>
       </c>
       <c r="E117" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F117" t="s">
         <v>0</v>
@@ -3421,22 +3394,22 @@
         <v>59</v>
       </c>
       <c r="B118" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C118" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D118" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E118" t="s">
-        <v>161</v>
+        <v>93</v>
       </c>
       <c r="F118" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G118" t="s">
-        <v>216</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119">
@@ -3447,13 +3420,13 @@
         <v>0</v>
       </c>
       <c r="C119" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D119" t="s">
         <v>0</v>
       </c>
       <c r="E119" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F119" t="s">
         <v>0</v>
@@ -3467,22 +3440,22 @@
         <v>60</v>
       </c>
       <c r="B120" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C120" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D120" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E120" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="F120" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G120" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="121">
@@ -3493,13 +3466,13 @@
         <v>0</v>
       </c>
       <c r="C121" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D121" t="s">
         <v>0</v>
       </c>
       <c r="E121" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F121" t="s">
         <v>0</v>
@@ -3513,22 +3486,22 @@
         <v>61</v>
       </c>
       <c r="B122" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C122" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="D122" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E122" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F122" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G122" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="123">
@@ -3539,13 +3512,13 @@
         <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D123" t="s">
         <v>0</v>
       </c>
       <c r="E123" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="F123" t="s">
         <v>0</v>
@@ -3559,251 +3532,21 @@
         <v>62</v>
       </c>
       <c r="B124" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D124" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="E124" t="s">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="F124" t="s">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="G124" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="s">
-        <v>0</v>
-      </c>
-      <c r="B125" t="s">
-        <v>0</v>
-      </c>
-      <c r="C125" t="s">
-        <v>80</v>
-      </c>
-      <c r="D125" t="s">
-        <v>0</v>
-      </c>
-      <c r="E125" t="s">
-        <v>80</v>
-      </c>
-      <c r="F125" t="s">
-        <v>0</v>
-      </c>
-      <c r="G125" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="s">
-        <v>63</v>
-      </c>
-      <c r="B126" t="s">
-        <v>70</v>
-      </c>
-      <c r="C126" t="s">
-        <v>98</v>
-      </c>
-      <c r="D126" t="s">
-        <v>129</v>
-      </c>
-      <c r="E126" t="s">
-        <v>98</v>
-      </c>
-      <c r="F126" t="s">
-        <v>174</v>
-      </c>
-      <c r="G126" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" t="s">
-        <v>0</v>
-      </c>
-      <c r="C127" t="s">
-        <v>88</v>
-      </c>
-      <c r="D127" t="s">
-        <v>0</v>
-      </c>
-      <c r="E127" t="s">
-        <v>88</v>
-      </c>
-      <c r="F127" t="s">
-        <v>0</v>
-      </c>
-      <c r="G127" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s">
-        <v>64</v>
-      </c>
-      <c r="B128" t="s">
-        <v>70</v>
-      </c>
-      <c r="C128" t="s">
-        <v>124</v>
-      </c>
-      <c r="D128" t="s">
-        <v>129</v>
-      </c>
-      <c r="E128" t="s">
-        <v>100</v>
-      </c>
-      <c r="F128" t="s">
-        <v>174</v>
-      </c>
-      <c r="G128" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="s">
-        <v>0</v>
-      </c>
-      <c r="B129" t="s">
-        <v>0</v>
-      </c>
-      <c r="C129" t="s">
-        <v>88</v>
-      </c>
-      <c r="D129" t="s">
-        <v>0</v>
-      </c>
-      <c r="E129" t="s">
-        <v>80</v>
-      </c>
-      <c r="F129" t="s">
-        <v>0</v>
-      </c>
-      <c r="G129" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="s">
-        <v>65</v>
-      </c>
-      <c r="B130" t="s">
-        <v>70</v>
-      </c>
-      <c r="C130" t="s">
-        <v>125</v>
-      </c>
-      <c r="D130" t="s">
-        <v>129</v>
-      </c>
-      <c r="E130" t="s">
-        <v>170</v>
-      </c>
-      <c r="F130" t="s">
-        <v>174</v>
-      </c>
-      <c r="G130" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="s">
-        <v>0</v>
-      </c>
-      <c r="B131" t="s">
-        <v>0</v>
-      </c>
-      <c r="C131" t="s">
-        <v>80</v>
-      </c>
-      <c r="D131" t="s">
-        <v>0</v>
-      </c>
-      <c r="E131" t="s">
-        <v>80</v>
-      </c>
-      <c r="F131" t="s">
-        <v>0</v>
-      </c>
-      <c r="G131" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="s">
-        <v>66</v>
-      </c>
-      <c r="B132" t="s">
-        <v>70</v>
-      </c>
-      <c r="C132" t="s">
-        <v>126</v>
-      </c>
-      <c r="D132" t="s">
-        <v>129</v>
-      </c>
-      <c r="E132" t="s">
-        <v>171</v>
-      </c>
-      <c r="F132" t="s">
-        <v>174</v>
-      </c>
-      <c r="G132" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="s">
-        <v>0</v>
-      </c>
-      <c r="B133" t="s">
-        <v>0</v>
-      </c>
-      <c r="C133" t="s">
-        <v>127</v>
-      </c>
-      <c r="D133" t="s">
-        <v>0</v>
-      </c>
-      <c r="E133" t="s">
-        <v>172</v>
-      </c>
-      <c r="F133" t="s">
-        <v>0</v>
-      </c>
-      <c r="G133" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="s">
-        <v>67</v>
-      </c>
-      <c r="B134" t="s">
-        <v>0</v>
-      </c>
-      <c r="C134" t="s">
-        <v>0</v>
-      </c>
-      <c r="D134" t="s">
-        <v>0</v>
-      </c>
-      <c r="E134" t="s">
-        <v>0</v>
-      </c>
-      <c r="F134" t="s">
-        <v>0</v>
-      </c>
-      <c r="G134" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>